<commit_message>
Read ratings from excel
</commit_message>
<xml_diff>
--- a/tests/reader/full_5_0_6.xlsx
+++ b/tests/reader/full_5_0_6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="0. Intro" sheetId="1" state="visible" r:id="rId2"/>
@@ -15216,7 +15216,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15312,7 +15312,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.000799999999999985</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -15321,11 +15321,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="94617126"/>
-        <c:axId val="54163501"/>
+        <c:axId val="17776772"/>
+        <c:axId val="35119663"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="94617126"/>
+        <c:axId val="17776772"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -15365,7 +15365,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54163501"/>
+        <c:crossAx val="35119663"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15373,7 +15373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54163501"/>
+        <c:axId val="35119663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15417,7 +15417,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94617126"/>
+        <c:crossAx val="17776772"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -15446,7 +15446,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15557,11 +15557,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="34841155"/>
-        <c:axId val="80809894"/>
+        <c:axId val="64396805"/>
+        <c:axId val="17460509"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="34841155"/>
+        <c:axId val="64396805"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -15601,7 +15601,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80809894"/>
+        <c:crossAx val="17460509"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15609,7 +15609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80809894"/>
+        <c:axId val="17460509"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15653,7 +15653,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34841155"/>
+        <c:crossAx val="64396805"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -15682,7 +15682,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15874,7 +15874,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.05</c:v>
@@ -15883,11 +15883,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="4909214"/>
-        <c:axId val="8453503"/>
+        <c:axId val="12999416"/>
+        <c:axId val="72741211"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="4909214"/>
+        <c:axId val="12999416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -15927,7 +15927,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8453503"/>
+        <c:crossAx val="72741211"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15935,7 +15935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8453503"/>
+        <c:axId val="72741211"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15979,7 +15979,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4909214"/>
+        <c:crossAx val="12999416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -16357,8 +16357,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41550,8 +41550,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42197,10 +42197,10 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42280,11 +42280,11 @@
       <c r="G4" s="73"/>
       <c r="H4" s="74" t="n">
         <f aca="false">I4/J4</f>
-        <v>-0.389047619047619</v>
+        <v>-0.377619047619048</v>
       </c>
       <c r="I4" s="75" t="n">
         <f aca="false">IF(SUM(I9+I23+I38+I59+I76)*1000/SUM(J9+J23+J38+J59+J76)&lt;-3600,-3600,SUM(I9+I23+I38+I59+I76)*1000/SUM(J9+J23+J38+J59+J76))</f>
-        <v>-389.047619047619</v>
+        <v>-377.619047619048</v>
       </c>
       <c r="J4" s="76" t="n">
         <f aca="false">SUM(J9+J23+J38+J59+J76)*1000/SUM(J9+J23+J38+J59+J76)</f>
@@ -45474,11 +45474,11 @@
       <c r="G76" s="116"/>
       <c r="H76" s="93" t="n">
         <f aca="false">IFERROR(I76/J76,0)</f>
-        <v>-0.50875</v>
+        <v>-0.44875</v>
       </c>
       <c r="I76" s="94" t="n">
         <f aca="false">I77+I81+I86+I90</f>
-        <v>-96.9047619047619</v>
+        <v>-85.4761904761905</v>
       </c>
       <c r="J76" s="94" t="n">
         <f aca="false">J77+J81+J86+J90</f>
@@ -45913,11 +45913,11 @@
       <c r="G86" s="112"/>
       <c r="H86" s="101" t="n">
         <f aca="false">IF(J86&lt;&gt;0,SUM(I87:I89)/J86,"-")</f>
-        <v>-0.06</v>
+        <v>0.18</v>
       </c>
       <c r="I86" s="102" t="n">
         <f aca="false">IF(J86=0,0,H86*J86)</f>
-        <v>-2.85714285714286</v>
+        <v>8.57142857142857</v>
       </c>
       <c r="J86" s="102" t="n">
         <f aca="false">'9. Weighting'!O42</f>
@@ -45973,7 +45973,7 @@
       </c>
       <c r="J87" s="110" t="n">
         <f aca="false">IFERROR(J86*K87/SUM($K$87:$K$88),0)</f>
-        <v>23.8095238095238</v>
+        <v>19.047619047619</v>
       </c>
       <c r="K87" s="1" t="n">
         <f aca="false">VLOOKUP(D87,$C$102:$E$106,3,FALSE())</f>
@@ -46006,30 +46006,31 @@
         <v>Relative impact</v>
       </c>
       <c r="D88" s="104" t="n">
-        <f aca="false">C104</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E88" s="113" t="str">
         <f aca="false">VLOOKUP(D88,$C$102:$D$106,2,FALSE())</f>
-        <v>medium</v>
+        <v>high</v>
       </c>
       <c r="F88" s="106" t="str">
         <f aca="false">'12.lan'!$D$329</f>
         <v>Introduce value between 0 and 10</v>
       </c>
       <c r="G88" s="107"/>
-      <c r="H88" s="108"/>
+      <c r="H88" s="108" t="n">
+        <v>4</v>
+      </c>
       <c r="I88" s="109" t="n">
         <f aca="false">IFERROR(J88*H88/10,0)</f>
-        <v>0</v>
+        <v>11.4285714285714</v>
       </c>
       <c r="J88" s="110" t="n">
         <f aca="false">IFERROR(J86*K88/SUM($K$87:$K$88),0)</f>
-        <v>23.8095238095238</v>
+        <v>28.5714285714286</v>
       </c>
       <c r="K88" s="1" t="n">
         <f aca="false">VLOOKUP(D88,$C$102:$E$106,3,FALSE())</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="L88" s="1" t="n">
         <f aca="false">VLOOKUP(O88,$C$102:$E$106,3,FALSE())</f>
@@ -46037,11 +46038,11 @@
       </c>
       <c r="M88" s="1" t="n">
         <f aca="false">VLOOKUP(D88,$C$102:$E$106,3,FALSE())</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N88" s="46" t="str">
         <f aca="false">IF(L88=M88,"",'12.lan'!$D$240&amp;VLOOKUP(L88,$C$102:$D$106,2,FALSE())&amp;" ("&amp;L88&amp;")")</f>
-        <v/>
+        <v>Weighting changed. Original medium (1)</v>
       </c>
       <c r="O88" s="1" t="n">
         <f aca="false">C104</f>
@@ -46284,11 +46285,11 @@
       <c r="G95" s="130"/>
       <c r="H95" s="131" t="n">
         <f aca="false">H4</f>
-        <v>-0.389047619047619</v>
+        <v>-0.377619047619048</v>
       </c>
       <c r="I95" s="132" t="n">
         <f aca="false">I4</f>
-        <v>-389.047619047619</v>
+        <v>-377.619047619048</v>
       </c>
       <c r="J95" s="132" t="n">
         <f aca="false">J4</f>
@@ -49932,7 +49933,7 @@
       <c r="J4" s="317"/>
       <c r="K4" s="318" t="n">
         <f aca="false">'3. Calc'!I4</f>
-        <v>-389.047619047619</v>
+        <v>-377.619047619048</v>
       </c>
       <c r="L4" s="318"/>
       <c r="M4" s="319" t="str">
@@ -50508,7 +50509,7 @@
       </c>
       <c r="K17" s="327" t="n">
         <f aca="false">'3. Calc'!I86</f>
-        <v>-2.85714285714286</v>
+        <v>8.57142857142857</v>
       </c>
       <c r="L17" s="328" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -50520,7 +50521,7 @@
       </c>
       <c r="N17" s="330" t="n">
         <f aca="false">'3. Calc'!H86</f>
-        <v>-0.06</v>
+        <v>0.18</v>
       </c>
       <c r="O17" s="327" t="n">
         <f aca="false">'3. Calc'!I90</f>
@@ -50830,7 +50831,7 @@
       </c>
       <c r="C20" s="350" t="n">
         <f aca="false">'4. ECG-Matrix'!K9+'4. ECG-Matrix'!K11+'4. ECG-Matrix'!K13+'4. ECG-Matrix'!K15+'4. ECG-Matrix'!K17</f>
-        <v>-11.1904761904762</v>
+        <v>0.238095238095234</v>
       </c>
       <c r="D20" s="351" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -50842,11 +50843,11 @@
       </c>
       <c r="F20" s="353" t="n">
         <f aca="false">C20/E20</f>
-        <v>-0.0376</v>
+        <v>0.000799999999999985</v>
       </c>
       <c r="G20" s="354" t="n">
         <f aca="false">IF(F20&lt;0,0,F20)</f>
-        <v>0</v>
+        <v>0.000799999999999985</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -50884,7 +50885,7 @@
       </c>
       <c r="C22" s="356" t="n">
         <f aca="false">'3. Calc'!I4</f>
-        <v>-389.047619047619</v>
+        <v>-377.619047619048</v>
       </c>
       <c r="D22" s="357" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -50896,7 +50897,7 @@
       </c>
       <c r="F22" s="359" t="n">
         <f aca="false">C22/E22</f>
-        <v>-0.389047619047619</v>
+        <v>-0.377619047619048</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -51220,7 +51221,7 @@
       </c>
       <c r="C22" s="350" t="n">
         <f aca="false">'3. Calc'!I76</f>
-        <v>-96.9047619047619</v>
+        <v>-85.4761904761905</v>
       </c>
       <c r="D22" s="351" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -51232,7 +51233,7 @@
       </c>
       <c r="F22" s="353" t="n">
         <f aca="false">C22/E22</f>
-        <v>-0.50875</v>
+        <v>-0.44875</v>
       </c>
       <c r="G22" s="354" t="n">
         <f aca="false">IF(F22&lt;0,0,F22)</f>
@@ -51247,7 +51248,7 @@
       </c>
       <c r="C23" s="356" t="n">
         <f aca="false">'3. Calc'!I4</f>
-        <v>-389.047619047619</v>
+        <v>-377.619047619048</v>
       </c>
       <c r="D23" s="357" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -51259,7 +51260,7 @@
       </c>
       <c r="F23" s="359" t="n">
         <f aca="false">C23/E23</f>
-        <v>-0.389047619047619</v>
+        <v>-0.377619047619048</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -51982,7 +51983,7 @@
       </c>
       <c r="C36" s="350" t="n">
         <f aca="false">'4. ECG-Matrix'!K17</f>
-        <v>-2.85714285714286</v>
+        <v>8.57142857142857</v>
       </c>
       <c r="D36" s="351" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -51994,11 +51995,11 @@
       </c>
       <c r="F36" s="360" t="n">
         <f aca="false">C36/E36</f>
-        <v>-0.06</v>
+        <v>0.18</v>
       </c>
       <c r="G36" s="354" t="n">
         <f aca="false">IF(F36&lt;0,0,F36)</f>
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AI36" s="361"/>
       <c r="AM36" s="361"/>
@@ -52039,7 +52040,7 @@
       </c>
       <c r="C38" s="356" t="n">
         <f aca="false">'3. Calc'!I4</f>
-        <v>-389.047619047619</v>
+        <v>-377.619047619048</v>
       </c>
       <c r="D38" s="362" t="str">
         <f aca="false">'12.lan'!$D$214</f>
@@ -52051,7 +52052,7 @@
       </c>
       <c r="F38" s="363" t="n">
         <f aca="false">C38/E38</f>
-        <v>-0.389047619047619</v>
+        <v>-0.377619047619048</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Handle undefined values in excel
</commit_message>
<xml_diff>
--- a/tests/reader/full_5_0_6.xlsx
+++ b/tests/reader/full_5_0_6.xlsx
@@ -15216,7 +15216,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15321,11 +15321,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="17776772"/>
-        <c:axId val="35119663"/>
+        <c:axId val="61695323"/>
+        <c:axId val="70556186"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="17776772"/>
+        <c:axId val="61695323"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -15365,7 +15365,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35119663"/>
+        <c:crossAx val="70556186"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15373,7 +15373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35119663"/>
+        <c:axId val="70556186"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15417,7 +15417,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17776772"/>
+        <c:crossAx val="61695323"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -15446,7 +15446,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15557,11 +15557,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64396805"/>
-        <c:axId val="17460509"/>
+        <c:axId val="39071451"/>
+        <c:axId val="72181052"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="64396805"/>
+        <c:axId val="39071451"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -15601,7 +15601,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17460509"/>
+        <c:crossAx val="72181052"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15609,7 +15609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17460509"/>
+        <c:axId val="72181052"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15653,7 +15653,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64396805"/>
+        <c:crossAx val="39071451"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -15682,7 +15682,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15883,11 +15883,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="12999416"/>
-        <c:axId val="72741211"/>
+        <c:axId val="87593250"/>
+        <c:axId val="40113606"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="12999416"/>
+        <c:axId val="87593250"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -15927,7 +15927,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72741211"/>
+        <c:crossAx val="40113606"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15935,7 +15935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72741211"/>
+        <c:axId val="40113606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -15979,7 +15979,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12999416"/>
+        <c:crossAx val="87593250"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -16357,8 +16357,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42197,10 +42197,10 @@
   </sheetPr>
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="N88" activeCellId="0" sqref="N88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>